<commit_message>
editing blue and red tank animations
</commit_message>
<xml_diff>
--- a/sheet drop.xlsx
+++ b/sheet drop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\AppData\Roaming\pico-8\carts\drop-p8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B05882-A293-43D9-B8D7-C4DD10CAF1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332D27D0-B570-43F1-87E2-22CD8B77D281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="750" windowWidth="19440" windowHeight="15000" xr2:uid="{2F517386-D81F-4AF1-A133-9D983E9345C9}"/>
   </bookViews>
@@ -163,7 +163,7 @@
     <t>{64,-10,-40,32,64,140}</t>
   </si>
   <si>
-    <t>{64,168,32,64,140}</t>
+    <t>{64,-10,168,32,64,140}</t>
   </si>
 </sst>
 </file>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968E7FE8-EAA6-4D7C-962A-12CADC7F5F87}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +652,7 @@
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
     <col min="6" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -1061,8 +1061,8 @@
         <v>41</v>
       </c>
       <c r="E21" s="6" t="str">
-        <f t="shared" ref="E21:E23" si="2">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A21:D21),"},")</f>
-        <v>{5,64,64,{64,168,32,64,140}},</v>
+        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A21:D21),"}")</f>
+        <v>{5,64,64,{64,-10,168,32,64,140}}</v>
       </c>
       <c r="F21" t="s">
         <v>36</v>
@@ -1113,7 +1113,7 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN("",TRUE,E17:E21),"},")</f>
-        <v>{{2,64,64},{3,0,10},{4,48,80},{5,64,64,{64,-10,-40,32,64,140}},{5,64,64,{64,168,32,64,140}},},</v>
+        <v>{{2,64,64},{3,0,10},{4,48,80},{5,64,64,{64,-10,-40,32,64,140}},{5,64,64,{64,-10,168,32,64,140}}},</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1181,7 +1181,7 @@
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
       <c r="E31" s="6" t="str">
-        <f t="shared" ref="E31:E35" si="3">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A31:C31),"},")</f>
+        <f t="shared" ref="E31:E35" si="2">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A31:C31),"},")</f>
         <v>{},</v>
       </c>
     </row>
@@ -1191,7 +1191,7 @@
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{},</v>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{},</v>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
       <c r="E34" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{},</v>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{},</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update level print and animations
</commit_message>
<xml_diff>
--- a/sheet drop.xlsx
+++ b/sheet drop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\AppData\Roaming\pico-8\carts\drop-p8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332D27D0-B570-43F1-87E2-22CD8B77D281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76B531D-44B4-460F-AF5F-AC7A20CE54B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="750" windowWidth="19440" windowHeight="15000" xr2:uid="{2F517386-D81F-4AF1-A133-9D983E9345C9}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t>sx</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>{64,-10,168,32,64,140}</t>
+  </si>
+  <si>
+    <t>every 10 b_points gives mult</t>
+  </si>
+  <si>
+    <t>fruitlet</t>
+  </si>
+  <si>
+    <t>blue</t>
   </si>
 </sst>
 </file>
@@ -644,7 +653,7 @@
   <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,6 +993,9 @@
       <c r="F17" t="s">
         <v>36</v>
       </c>
+      <c r="G17" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -1043,6 +1055,12 @@
       <c r="F20" t="s">
         <v>36</v>
       </c>
+      <c r="G20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
       <c r="J20" t="s">
         <v>25</v>
       </c>
@@ -1066,6 +1084,9 @@
       </c>
       <c r="F21" t="s">
         <v>36</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
       </c>
       <c r="J21" t="s">
         <v>29</v>
@@ -1079,6 +1100,12 @@
       <c r="E22" s="6"/>
       <c r="F22" t="s">
         <v>36</v>
+      </c>
+      <c r="G22" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
       </c>
       <c r="J22" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
worked on end of level scene
</commit_message>
<xml_diff>
--- a/sheet drop.xlsx
+++ b/sheet drop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\AppData\Roaming\pico-8\carts\drop-p8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76B531D-44B4-460F-AF5F-AC7A20CE54B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F153C4-E172-4490-B22B-D70F1E357D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="750" windowWidth="19440" windowHeight="15000" xr2:uid="{2F517386-D81F-4AF1-A133-9D983E9345C9}"/>
   </bookViews>
@@ -302,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -314,8 +314,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,7 +651,7 @@
   <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,13 +683,13 @@
       <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -711,13 +709,12 @@
       <c r="A3" s="5">
         <v>0</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3">
         <v>8</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3">
         <v>64</v>
       </c>
-      <c r="D3" s="11"/>
       <c r="E3" s="6" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A3:C3),"},")</f>
         <v>{0,8,64},</v>
@@ -736,13 +733,12 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4">
         <v>64</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4">
         <v>120</v>
       </c>
-      <c r="D4" s="11"/>
       <c r="E4" s="6" t="str">
         <f t="shared" ref="E4:E8" si="0">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A4:C4),"},")</f>
         <v>{1,64,120},</v>
@@ -761,13 +757,12 @@
       <c r="A5" s="5">
         <v>0</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5">
         <v>8</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5">
         <v>64</v>
       </c>
-      <c r="D5" s="11"/>
       <c r="E5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>{0,8,64},</v>
@@ -789,13 +784,12 @@
       <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6">
         <v>64</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6">
         <v>120</v>
       </c>
-      <c r="D6" s="11"/>
       <c r="E6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>{1,64,120},</v>
@@ -817,13 +811,12 @@
       <c r="A7" s="5">
         <v>0</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7">
         <v>8</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7">
         <v>64</v>
       </c>
-      <c r="D7" s="11"/>
       <c r="E7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>{0,8,64},</v>
@@ -842,13 +835,12 @@
       <c r="A8" s="5">
         <v>1</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8">
         <v>64</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8">
         <v>120</v>
       </c>
-      <c r="D8" s="11"/>
       <c r="E8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>{1,64,120},</v>
@@ -867,13 +859,12 @@
       <c r="A9" s="5">
         <v>0</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9">
         <v>64</v>
       </c>
-      <c r="D9" s="11"/>
       <c r="E9" s="6" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A9:C9),"}")</f>
         <v>{0,8,64}</v>
@@ -890,9 +881,6 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -900,9 +888,6 @@
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN("",TRUE,E3:E9),"},")</f>
         <v>{{0,8,64},{1,64,120},{0,8,64},{1,64,120},{0,8,64},{1,64,120},{0,8,64}},</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
       <c r="E11" s="6"/>
       <c r="F11" t="s">
         <v>36</v>
@@ -959,13 +944,13 @@
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -979,13 +964,12 @@
       <c r="A17" s="5">
         <v>2</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17">
         <v>64</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17">
         <v>64</v>
       </c>
-      <c r="D17" s="11"/>
       <c r="E17" s="6" t="str">
         <f t="shared" ref="E17:E19" si="1">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A17:D17),"},")</f>
         <v>{2,64,64},</v>
@@ -1001,13 +985,12 @@
       <c r="A18" s="5">
         <v>3</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18">
         <v>0</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18">
         <v>10</v>
       </c>
-      <c r="D18" s="11"/>
       <c r="E18" s="6" t="str">
         <f t="shared" si="1"/>
         <v>{3,0,10},</v>
@@ -1020,13 +1003,12 @@
       <c r="A19" s="5">
         <v>4</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19">
         <v>48</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19">
         <v>80</v>
       </c>
-      <c r="D19" s="11"/>
       <c r="E19" s="6" t="str">
         <f t="shared" si="1"/>
         <v>{4,48,80},</v>
@@ -1039,13 +1021,13 @@
       <c r="A20" s="5">
         <v>5</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20">
         <v>64</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20">
         <v>64</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" t="s">
         <v>40</v>
       </c>
       <c r="E20" s="6" t="str">
@@ -1069,13 +1051,13 @@
       <c r="A21" s="5">
         <v>5</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21">
         <v>64</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21">
         <v>64</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" t="s">
         <v>41</v>
       </c>
       <c r="E21" s="6" t="str">
@@ -1094,9 +1076,6 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
       <c r="E22" s="6"/>
       <c r="F22" t="s">
         <v>36</v>
@@ -1113,9 +1092,6 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
       <c r="E23" s="6"/>
       <c r="F23" t="s">
         <v>36</v>
@@ -1126,9 +1102,6 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
       <c r="E24" s="6"/>
       <c r="F24" t="s">
         <v>36</v>
@@ -1179,13 +1152,13 @@
       <c r="A29" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" t="s">
         <v>32</v>
       </c>
       <c r="E29" s="6" t="s">
@@ -1194,9 +1167,6 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
       <c r="E30" s="6" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A30:C30),"},")</f>
         <v>{},</v>
@@ -1204,9 +1174,6 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
       <c r="E31" s="6" t="str">
         <f t="shared" ref="E31:E35" si="2">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A31:C31),"},")</f>
         <v>{},</v>
@@ -1214,9 +1181,6 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
       <c r="E32" s="6" t="str">
         <f t="shared" si="2"/>
         <v>{},</v>
@@ -1224,9 +1188,6 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
       <c r="E33" s="6" t="str">
         <f t="shared" si="2"/>
         <v>{},</v>
@@ -1234,9 +1195,6 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
       <c r="E34" s="6" t="str">
         <f t="shared" si="2"/>
         <v>{},</v>
@@ -1244,9 +1202,6 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
       <c r="E35" s="6" t="str">
         <f t="shared" si="2"/>
         <v>{},</v>
@@ -1254,9 +1209,6 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
       <c r="E36" s="6" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A36:C36),"}")</f>
         <v>{}</v>
@@ -1264,9 +1216,6 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
       <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed battery at low fuel
</commit_message>
<xml_diff>
--- a/sheet drop.xlsx
+++ b/sheet drop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\AppData\Roaming\pico-8\carts\drop-p8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F952E2-695A-40D1-9487-6EBBEC0A7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5017606E-F4D8-4ADD-B0AA-21D0266F2885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="750" windowWidth="19440" windowHeight="15000" xr2:uid="{2F517386-D81F-4AF1-A133-9D983E9345C9}"/>
   </bookViews>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968E7FE8-EAA6-4D7C-962A-12CADC7F5F87}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
shortened fruit pattern logic
</commit_message>
<xml_diff>
--- a/sheet drop.xlsx
+++ b/sheet drop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\AppData\Roaming\pico-8\carts\drop-p8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5017606E-F4D8-4ADD-B0AA-21D0266F2885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E89C5E-4AE9-4413-97F8-4C1F4FC3F736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="750" windowWidth="19440" windowHeight="15000" xr2:uid="{2F517386-D81F-4AF1-A133-9D983E9345C9}"/>
   </bookViews>
@@ -348,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -361,7 +361,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -700,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968E7FE8-EAA6-4D7C-962A-12CADC7F5F87}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,17 +756,17 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E3" s="12" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A3:C3),"},")</f>
-        <v>{8,0,0},</v>
+        <v>{9,80,80},</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -784,14 +783,14 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E4" s="12" t="str">
-        <f t="shared" ref="E4:E8" si="0">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A4:C4),"},")</f>
-        <v>{7,0,0},</v>
+        <f t="shared" ref="E4:E7" si="0">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A4:C4),"},")</f>
+        <v>{7,80,80},</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -882,7 +881,15 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="5">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <v>80</v>
+      </c>
       <c r="E8" s="12"/>
       <c r="G8">
         <v>5</v>
@@ -895,7 +902,15 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <v>80</v>
+      </c>
       <c r="E9" s="12"/>
       <c r="G9">
         <v>6</v>
@@ -909,7 +924,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="12"/>
       <c r="G10">
         <v>7</v>
       </c>
@@ -923,9 +938,9 @@
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN("",TRUE,E3:E9),"},")</f>
-        <v>{{8,0,0},{7,0,0},{0,8,64},{1,64,120},{0,8,64},},</v>
-      </c>
-      <c r="E11" s="13"/>
+        <v>{{9,80,80},{7,80,80},{0,8,64},{1,64,120},{0,8,64},},</v>
+      </c>
+      <c r="E11" s="12"/>
       <c r="F11" t="s">
         <v>36</v>
       </c>
@@ -944,7 +959,7 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="14"/>
+      <c r="E12" s="13"/>
       <c r="F12" t="s">
         <v>36</v>
       </c>
@@ -1116,7 +1131,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="12"/>
       <c r="F22" t="s">
         <v>36</v>
       </c>
@@ -1132,7 +1147,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="E23" s="13"/>
+      <c r="E23" s="12"/>
       <c r="F23" t="s">
         <v>36</v>
       </c>
@@ -1145,7 +1160,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="E24" s="13"/>
+      <c r="E24" s="12"/>
       <c r="F24" t="s">
         <v>36</v>
       </c>
@@ -1167,7 +1182,7 @@
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="14"/>
+      <c r="E25" s="13"/>
       <c r="F25" t="s">
         <v>36</v>
       </c>
@@ -1216,62 +1231,62 @@
       <c r="D29" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="E30" s="13" t="str">
+      <c r="E30" s="12" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A30:C30),"},")</f>
         <v>{},</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="E31" s="13" t="str">
+      <c r="E31" s="12" t="str">
         <f t="shared" ref="E31:E35" si="2">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A31:C31),"},")</f>
         <v>{},</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="E32" s="13" t="str">
+      <c r="E32" s="12" t="str">
         <f t="shared" si="2"/>
         <v>{},</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="E33" s="13" t="str">
+      <c r="E33" s="12" t="str">
         <f t="shared" si="2"/>
         <v>{},</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="E34" s="13" t="str">
+      <c r="E34" s="12" t="str">
         <f t="shared" si="2"/>
         <v>{},</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="E35" s="13" t="str">
+      <c r="E35" s="12" t="str">
         <f t="shared" si="2"/>
         <v>{},</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="E36" s="13" t="str">
+      <c r="E36" s="12" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A36:C36),"}")</f>
         <v>{}</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="E37" s="13"/>
+      <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="str">
@@ -1281,7 +1296,7 @@
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="14"/>
+      <c r="E38" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed dots looking off
</commit_message>
<xml_diff>
--- a/sheet drop.xlsx
+++ b/sheet drop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\AppData\Roaming\pico-8\carts\drop-p8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F13942-CFD4-4D97-B62B-5A1831FC43EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A9C041-B97A-4C25-B956-8974ABCEFEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="855" windowWidth="19440" windowHeight="15000" xr2:uid="{2F517386-D81F-4AF1-A133-9D983E9345C9}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
   <si>
     <t>sx</t>
   </si>
@@ -97,12 +97,6 @@
     <t>cubic bezier</t>
   </si>
   <si>
-    <t>zigr</t>
-  </si>
-  <si>
-    <t>zigl</t>
-  </si>
-  <si>
     <t>wave_info (sx,ex,bez_arr)</t>
   </si>
   <si>
@@ -188,6 +182,21 @@
   </si>
   <si>
     <t>default ex</t>
+  </si>
+  <si>
+    <t>zig l</t>
+  </si>
+  <si>
+    <t>zig r</t>
+  </si>
+  <si>
+    <t>curves</t>
+  </si>
+  <si>
+    <t>staggered</t>
+  </si>
+  <si>
+    <t>crossing</t>
   </si>
 </sst>
 </file>
@@ -706,7 +715,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="A19" sqref="A19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,28 +736,30 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>12</v>
@@ -757,76 +768,91 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="E3" s="12" t="str">
-        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A3:C3),"},")</f>
-        <v>{9,80,80},</v>
+        <f t="shared" ref="E3:E4" si="0">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A3:D3),"},")</f>
+        <v>{0,8,64},</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="I3">
         <v>10</v>
       </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>64</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C4">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="E4" s="12" t="str">
-        <f t="shared" ref="E4:E9" si="0">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A4:C4),"},")</f>
-        <v>{7,80,80},</v>
+        <f t="shared" si="0"/>
+        <v>{1,64,120},</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
+      <c r="J4">
+        <v>64</v>
+      </c>
+      <c r="K4">
+        <v>120</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>64</v>
       </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
       <c r="E5" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>{0,8,64},</v>
+        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A5:D5),"},")</f>
+        <v>{5,32,64,{64,-10,-40,32,64,140}},</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -846,17 +872,20 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6">
         <v>64</v>
       </c>
-      <c r="C6">
-        <v>120</v>
+      <c r="D6" t="s">
+        <v>38</v>
       </c>
       <c r="E6" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>{1,64,120},</v>
+        <f t="shared" ref="E6:E9" si="1">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A6:D6),"},")</f>
+        <v>{5,32,64,{64,-10,168,32,64,140}},</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -867,20 +896,26 @@
       <c r="I6">
         <v>5</v>
       </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C7">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="E7" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>{0,8,64},</v>
+        <f t="shared" si="1"/>
+        <v>{1,64,120},</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -891,20 +926,26 @@
       <c r="I7">
         <v>20</v>
       </c>
+      <c r="J7">
+        <v>40</v>
+      </c>
+      <c r="K7">
+        <v>80</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="E8" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>{9,80,80},</v>
+        <f t="shared" si="1"/>
+        <v>{0,8,64},</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -918,17 +959,17 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E9" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>{7,80,80},</v>
+        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A9:D9),"}")</f>
+        <v>{3,0,0}</v>
       </c>
       <c r="G9">
         <v>6</v>
@@ -947,29 +988,41 @@
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I10">
         <v>8</v>
       </c>
+      <c r="J10">
+        <v>80</v>
+      </c>
+      <c r="K10">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN("",TRUE,E3:E9),"},")</f>
-        <v>{{9,80,80},{7,80,80},{0,8,64},{1,64,120},{0,8,64},{9,80,80},{7,80,80},},</v>
+        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN("",TRUE,E3:E10),"},")</f>
+        <v>{{0,8,64},{1,64,120},{5,32,64,{64,-10,-40,32,64,140}},{5,32,64,{64,-10,168,32,64,140}},{1,64,120},{0,8,64},{3,0,0}},</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G11">
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I11">
         <v>8</v>
+      </c>
+      <c r="J11">
+        <v>80</v>
+      </c>
+      <c r="K11">
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -979,67 +1032,72 @@
       <c r="D12" s="8"/>
       <c r="E12" s="13"/>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G12">
         <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
+      <c r="J12">
+        <v>70</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13">
-        <v>10</v>
-      </c>
-      <c r="H13" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="11"/>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="F16" t="s">
         <v>33</v>
       </c>
-      <c r="F16" t="s">
-        <v>35</v>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1053,11 +1111,11 @@
         <v>60</v>
       </c>
       <c r="E17" s="12" t="str">
-        <f t="shared" ref="E17:E23" si="1">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A17:D17),"},")</f>
+        <f t="shared" ref="E17:E23" si="2">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A17:D17),"},")</f>
         <v>{2,0,60},</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1068,59 +1126,59 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E18" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>{3,0,10},</v>
+        <f t="shared" si="2"/>
+        <v>{3,0,0},</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C19">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E19" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>{2,0,60},</v>
+        <f t="shared" si="2"/>
+        <v>{4,40,80},</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E20" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>{3,0,10},</v>
+        <f t="shared" si="2"/>
+        <v>{2,0,60},</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
         <v>11</v>
@@ -1131,20 +1189,20 @@
         <v>4</v>
       </c>
       <c r="B21">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C21">
         <v>80</v>
       </c>
       <c r="E21" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>{4,48,80},</v>
+        <f t="shared" si="2"/>
+        <v>{4,40,80},</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1158,14 +1216,14 @@
         <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E22" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{5,32,64,{64,-10,-40,32,64,140}},</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1179,158 +1237,216 @@
         <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>{5,32,64,{64,-10,168,32,64,140}},</v>
+        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A23:D23),"}")</f>
+        <v>{5,32,64,{64,-10,168,32,64,140}}</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="E24" s="12"/>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN("",TRUE,E17:E24),"},")</f>
-        <v>{{2,0,60},{3,0,10},{2,0,60},{3,0,10},{4,48,80},{5,32,64,{64,-10,-40,32,64,140}},{5,32,64,{64,-10,168,32,64,140}},},</v>
+        <v>{{2,0,60},{3,0,0},{4,40,80},{2,0,60},{4,40,80},{5,32,64,{64,-10,-40,32,64,140}},{5,32,64,{64,-10,168,32,64,140}}},</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="13"/>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="11"/>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H28">
         <v>5</v>
       </c>
       <c r="J28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>33</v>
-      </c>
       <c r="G29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H29">
         <v>10</v>
       </c>
       <c r="J29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+      <c r="A30" s="5">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>80</v>
+      </c>
+      <c r="C30">
+        <v>80</v>
+      </c>
       <c r="E30" s="12" t="str">
-        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A30:C30),"},")</f>
-        <v>{},</v>
+        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A30:D30),"},")</f>
+        <v>{8,80,80},</v>
       </c>
       <c r="K30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>80</v>
+      </c>
+      <c r="C31">
+        <v>80</v>
+      </c>
+      <c r="E31" s="12" t="str">
+        <f t="shared" ref="E31:E36" si="3">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A31:D31),"},")</f>
+        <v>{7,80,80},</v>
+      </c>
+      <c r="K31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>70</v>
+      </c>
+      <c r="C32">
+        <v>100</v>
+      </c>
+      <c r="E32" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>{9,70,100},</v>
+      </c>
+      <c r="K32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="E31" s="12" t="str">
-        <f t="shared" ref="E31:E35" si="2">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A31:C31),"},")</f>
-        <v>{},</v>
-      </c>
-      <c r="K31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="E32" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{},</v>
-      </c>
-      <c r="K32" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
+      <c r="A33" s="5">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
       <c r="E33" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{},</v>
+        <f t="shared" si="3"/>
+        <v>{3,0,0},</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
+      <c r="A34" s="5">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>70</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
+      </c>
       <c r="E34" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{},</v>
+        <f t="shared" si="3"/>
+        <v>{9,70,100},</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
+      <c r="A35" s="5">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>80</v>
+      </c>
+      <c r="C35">
+        <v>80</v>
+      </c>
       <c r="E35" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{},</v>
+        <f t="shared" si="3"/>
+        <v>{8,80,80},</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
+      <c r="A36" s="5">
+        <v>7</v>
+      </c>
+      <c r="B36">
+        <v>80</v>
+      </c>
+      <c r="C36">
+        <v>80</v>
+      </c>
       <c r="E36" s="12" t="str">
-        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A36:C36),"}")</f>
-        <v>{}</v>
+        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A36:D36),"}")</f>
+        <v>{7,80,80}</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1340,7 +1456,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="str">
         <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN("",TRUE,E30:E36),"},")</f>
-        <v>{{},{},{},{},{},{},{}},</v>
+        <v>{{8,80,80},{7,80,80},{9,70,100},{3,0,0},{9,70,100},{8,80,80},{7,80,80}},</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>

</xml_diff>

<commit_message>
added cubic pattern back in
</commit_message>
<xml_diff>
--- a/sheet drop.xlsx
+++ b/sheet drop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\AppData\Roaming\pico-8\carts\drop-p8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A9C041-B97A-4C25-B956-8974ABCEFEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC110C7-6DD0-480D-8EBC-842848DF1257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="855" windowWidth="19440" windowHeight="15000" xr2:uid="{2F517386-D81F-4AF1-A133-9D983E9345C9}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
   <si>
     <t>sx</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>crossing</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>mixed</t>
+  </si>
+  <si>
+    <t>{64,-10,180,120,-60,120,64,-11}</t>
   </si>
 </sst>
 </file>
@@ -712,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968E7FE8-EAA6-4D7C-962A-12CADC7F5F87}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:C19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,6 +989,12 @@
       <c r="I9">
         <v>10</v>
       </c>
+      <c r="J9">
+        <v>64</v>
+      </c>
+      <c r="K9">
+        <v>64</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
@@ -1462,6 +1477,162 @@
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="13"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="E42" s="12" t="str">
+        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A42:D42),"},")</f>
+        <v>{3,0,0},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="12" t="str">
+        <f t="shared" ref="E43:E47" si="4">_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A43:D43),"},")</f>
+        <v>{6,0,0,{64,-10,180,120,-60,120,64,-11}},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>32</v>
+      </c>
+      <c r="C44">
+        <v>64</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>{5,32,64,{64,-10,-40,32,64,140}},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>32</v>
+      </c>
+      <c r="C45">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>{5,32,64,{64,-10,168,32,64,140}},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>70</v>
+      </c>
+      <c r="C46">
+        <v>100</v>
+      </c>
+      <c r="E46" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>{9,70,100},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>8</v>
+      </c>
+      <c r="B47">
+        <v>80</v>
+      </c>
+      <c r="C47">
+        <v>80</v>
+      </c>
+      <c r="E47" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>{8,80,80},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>7</v>
+      </c>
+      <c r="B48">
+        <v>80</v>
+      </c>
+      <c r="C48">
+        <v>80</v>
+      </c>
+      <c r="E48" s="12" t="str">
+        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN(",",TRUE,A48:D48),"}")</f>
+        <v>{7,80,80}</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="E49" s="12"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="str">
+        <f>_xlfn.CONCAT("{",_xlfn.TEXTJOIN("",TRUE,E42:E48),"},")</f>
+        <v>{{3,0,0},{6,0,0,{64,-10,180,120,-60,120,64,-11}},{5,32,64,{64,-10,-40,32,64,140}},{5,32,64,{64,-10,168,32,64,140}},{9,70,100},{8,80,80},{7,80,80}},</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>